<commit_message>
Noticed that some duration days were missing so filled those in
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2023_FilteringLog.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2023_FilteringLog.xlsx
@@ -14407,6 +14407,9 @@
       <c r="H324" s="5">
         <v>1.2</v>
       </c>
+      <c r="I324" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J324" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -14437,6 +14440,9 @@
       <c r="H325" s="5">
         <v>1.2</v>
       </c>
+      <c r="I325" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J325" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -14467,6 +14473,9 @@
       <c r="H326" s="5">
         <v>1.2</v>
       </c>
+      <c r="I326" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J326" s="5">
         <f t="shared" si="1"/>
         <v>0.004</v>
@@ -14497,7 +14506,9 @@
       <c r="H327" s="5">
         <v>1.2</v>
       </c>
-      <c r="I327" s="11"/>
+      <c r="I327" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J327" s="5">
         <f t="shared" si="1"/>
         <v>0.008</v>
@@ -14545,6 +14556,9 @@
       <c r="H328" s="5">
         <v>1.11</v>
       </c>
+      <c r="I328" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J328" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -14575,6 +14589,9 @@
       <c r="H329" s="5">
         <v>1.11</v>
       </c>
+      <c r="I329" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J329" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -14605,6 +14622,9 @@
       <c r="H330" s="5">
         <v>1.11</v>
       </c>
+      <c r="I330" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J330" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -14635,7 +14655,9 @@
       <c r="H331" s="5">
         <v>1.11</v>
       </c>
-      <c r="I331" s="11"/>
+      <c r="I331" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J331" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -14683,6 +14705,9 @@
       <c r="H332" s="5">
         <v>1.43</v>
       </c>
+      <c r="I332" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J332" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -14713,6 +14738,9 @@
       <c r="H333" s="5">
         <v>1.43</v>
       </c>
+      <c r="I333" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J333" s="5">
         <f t="shared" si="1"/>
         <v>0.017</v>
@@ -14743,6 +14771,9 @@
       <c r="H334" s="5">
         <v>1.43</v>
       </c>
+      <c r="I334" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J334" s="5">
         <f t="shared" si="1"/>
         <v>0.017</v>
@@ -14773,7 +14804,9 @@
       <c r="H335" s="5">
         <v>1.43</v>
       </c>
-      <c r="I335" s="11"/>
+      <c r="I335" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J335" s="5">
         <f t="shared" si="1"/>
         <v>0.017</v>
@@ -14821,6 +14854,9 @@
       <c r="H336" s="5">
         <v>1.52</v>
       </c>
+      <c r="I336" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J336" s="5">
         <f t="shared" si="1"/>
         <v>0.017</v>
@@ -14851,6 +14887,9 @@
       <c r="H337" s="5">
         <v>1.52</v>
       </c>
+      <c r="I337" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J337" s="5">
         <f t="shared" si="1"/>
         <v>0.017</v>
@@ -14881,6 +14920,9 @@
       <c r="H338" s="5">
         <v>1.52</v>
       </c>
+      <c r="I338" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J338" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -14911,7 +14953,9 @@
       <c r="H339" s="5">
         <v>1.52</v>
       </c>
-      <c r="I339" s="11"/>
+      <c r="I339" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J339" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -14959,6 +15003,9 @@
       <c r="H340" s="5">
         <v>1.16</v>
       </c>
+      <c r="I340" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J340" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -14989,6 +15036,9 @@
       <c r="H341" s="5">
         <v>1.16</v>
       </c>
+      <c r="I341" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J341" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -15019,6 +15069,9 @@
       <c r="H342" s="5">
         <v>1.16</v>
       </c>
+      <c r="I342" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J342" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -15049,7 +15102,9 @@
       <c r="H343" s="5">
         <v>1.16</v>
       </c>
-      <c r="I343" s="11"/>
+      <c r="I343" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J343" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -15097,6 +15152,9 @@
       <c r="H344" s="5">
         <v>1.155</v>
       </c>
+      <c r="I344" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J344" s="5">
         <f t="shared" si="1"/>
         <v>0.004</v>
@@ -15127,6 +15185,9 @@
       <c r="H345" s="5">
         <v>1.155</v>
       </c>
+      <c r="I345" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J345" s="5">
         <f t="shared" si="1"/>
         <v>0.003</v>
@@ -15157,6 +15218,9 @@
       <c r="H346" s="5">
         <v>1.155</v>
       </c>
+      <c r="I346" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J346" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -15187,7 +15251,9 @@
       <c r="H347" s="5">
         <v>1.155</v>
       </c>
-      <c r="I347" s="11"/>
+      <c r="I347" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J347" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -15235,6 +15301,9 @@
       <c r="H348" s="5">
         <v>1.4</v>
       </c>
+      <c r="I348" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J348" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -15265,6 +15334,9 @@
       <c r="H349" s="5">
         <v>1.4</v>
       </c>
+      <c r="I349" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J349" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -15295,6 +15367,9 @@
       <c r="H350" s="5">
         <v>1.4</v>
       </c>
+      <c r="I350" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J350" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -15325,7 +15400,9 @@
       <c r="H351" s="5">
         <v>1.4</v>
       </c>
-      <c r="I351" s="11"/>
+      <c r="I351" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J351" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -15373,6 +15450,9 @@
       <c r="H352" s="5">
         <v>1.395</v>
       </c>
+      <c r="I352" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J352" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -15403,6 +15483,9 @@
       <c r="H353" s="5">
         <v>1.395</v>
       </c>
+      <c r="I353" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J353" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -15433,6 +15516,9 @@
       <c r="H354" s="5">
         <v>1.395</v>
       </c>
+      <c r="I354" s="5">
+        <v>14.0</v>
+      </c>
       <c r="J354" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -15463,7 +15549,9 @@
       <c r="H355" s="5">
         <v>1.395</v>
       </c>
-      <c r="I355" s="11"/>
+      <c r="I355" s="8">
+        <v>14.0</v>
+      </c>
       <c r="J355" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -15511,6 +15599,9 @@
       <c r="H356" s="5">
         <v>1.105</v>
       </c>
+      <c r="I356" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J356" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -15541,6 +15632,9 @@
       <c r="H357" s="5">
         <v>1.105</v>
       </c>
+      <c r="I357" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J357" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -15571,6 +15665,9 @@
       <c r="H358" s="5">
         <v>1.105</v>
       </c>
+      <c r="I358" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J358" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -15601,7 +15698,9 @@
       <c r="H359" s="5">
         <v>1.105</v>
       </c>
-      <c r="I359" s="11"/>
+      <c r="I359" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J359" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -15649,6 +15748,9 @@
       <c r="H360" s="5">
         <v>1.2</v>
       </c>
+      <c r="I360" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J360" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -15679,6 +15781,9 @@
       <c r="H361" s="5">
         <v>1.2</v>
       </c>
+      <c r="I361" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J361" s="5">
         <f t="shared" si="1"/>
         <v>0.008</v>
@@ -15709,6 +15814,9 @@
       <c r="H362" s="5">
         <v>1.2</v>
       </c>
+      <c r="I362" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J362" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -15739,7 +15847,9 @@
       <c r="H363" s="5">
         <v>1.2</v>
       </c>
-      <c r="I363" s="11"/>
+      <c r="I363" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J363" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -15787,6 +15897,9 @@
       <c r="H364" s="5">
         <v>1.32</v>
       </c>
+      <c r="I364" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J364" s="5">
         <f t="shared" si="1"/>
         <v>0.021</v>
@@ -15817,6 +15930,9 @@
       <c r="H365" s="5">
         <v>1.32</v>
       </c>
+      <c r="I365" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J365" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -15847,6 +15963,9 @@
       <c r="H366" s="5">
         <v>1.32</v>
       </c>
+      <c r="I366" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J366" s="5">
         <f t="shared" si="1"/>
         <v>0.021</v>
@@ -15877,7 +15996,9 @@
       <c r="H367" s="5">
         <v>1.32</v>
       </c>
-      <c r="I367" s="11"/>
+      <c r="I367" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J367" s="5">
         <f t="shared" si="1"/>
         <v>0.019</v>
@@ -15927,6 +16048,9 @@
       <c r="H368" s="5">
         <v>1.305</v>
       </c>
+      <c r="I368" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J368" s="5">
         <f t="shared" si="1"/>
         <v>0.022</v>
@@ -15957,6 +16081,9 @@
       <c r="H369" s="5">
         <v>1.305</v>
       </c>
+      <c r="I369" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J369" s="5">
         <f t="shared" si="1"/>
         <v>0.02</v>
@@ -15987,6 +16114,9 @@
       <c r="H370" s="5">
         <v>1.305</v>
       </c>
+      <c r="I370" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J370" s="5">
         <f t="shared" si="1"/>
         <v>0.02</v>
@@ -16017,7 +16147,9 @@
       <c r="H371" s="8">
         <v>1.305</v>
       </c>
-      <c r="I371" s="11"/>
+      <c r="I371" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J371" s="5">
         <f t="shared" si="1"/>
         <v>0.018</v>
@@ -16065,6 +16197,9 @@
       <c r="H372" s="5">
         <v>1.14</v>
       </c>
+      <c r="I372" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J372" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16095,6 +16230,9 @@
       <c r="H373" s="5">
         <v>1.14</v>
       </c>
+      <c r="I373" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J373" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -16125,6 +16263,9 @@
       <c r="H374" s="5">
         <v>1.14</v>
       </c>
+      <c r="I374" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J374" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -16155,7 +16296,9 @@
       <c r="H375" s="8">
         <v>1.14</v>
       </c>
-      <c r="I375" s="11"/>
+      <c r="I375" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J375" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16203,6 +16346,9 @@
       <c r="H376" s="5">
         <v>1.155</v>
       </c>
+      <c r="I376" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J376" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16233,6 +16379,9 @@
       <c r="H377" s="5">
         <v>1.155</v>
       </c>
+      <c r="I377" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J377" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -16263,6 +16412,9 @@
       <c r="H378" s="5">
         <v>1.155</v>
       </c>
+      <c r="I378" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J378" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16293,7 +16445,9 @@
       <c r="H379" s="8">
         <v>1.155</v>
       </c>
-      <c r="I379" s="11"/>
+      <c r="I379" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J379" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16341,6 +16495,9 @@
       <c r="H380" s="5">
         <v>1.33</v>
       </c>
+      <c r="I380" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J380" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -16374,6 +16531,9 @@
       <c r="H381" s="5">
         <v>1.33</v>
       </c>
+      <c r="I381" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J381" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -16404,6 +16564,9 @@
       <c r="H382" s="5">
         <v>1.33</v>
       </c>
+      <c r="I382" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J382" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -16434,7 +16597,9 @@
       <c r="H383" s="8">
         <v>1.33</v>
       </c>
-      <c r="I383" s="11"/>
+      <c r="I383" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J383" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -16482,6 +16647,9 @@
       <c r="H384" s="5">
         <v>1.355</v>
       </c>
+      <c r="I384" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J384" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -16512,6 +16680,9 @@
       <c r="H385" s="5">
         <v>1.355</v>
       </c>
+      <c r="I385" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J385" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -16542,6 +16713,9 @@
       <c r="H386" s="5">
         <v>1.355</v>
       </c>
+      <c r="I386" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J386" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -16572,7 +16746,9 @@
       <c r="H387" s="8">
         <v>1.355</v>
       </c>
-      <c r="I387" s="11"/>
+      <c r="I387" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J387" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -16620,6 +16796,9 @@
       <c r="H388" s="5">
         <v>1.19</v>
       </c>
+      <c r="I388" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J388" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -16650,6 +16829,9 @@
       <c r="H389" s="5">
         <v>1.19</v>
       </c>
+      <c r="I389" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J389" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16680,6 +16862,9 @@
       <c r="H390" s="5">
         <v>1.19</v>
       </c>
+      <c r="I390" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J390" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -16710,7 +16895,9 @@
       <c r="H391" s="8">
         <v>1.19</v>
       </c>
-      <c r="I391" s="11"/>
+      <c r="I391" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J391" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16758,6 +16945,9 @@
       <c r="H392" s="5">
         <v>1.14</v>
       </c>
+      <c r="I392" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J392" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -16791,6 +16981,9 @@
       <c r="H393" s="5">
         <v>1.14</v>
       </c>
+      <c r="I393" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J393" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -16821,6 +17014,9 @@
       <c r="H394" s="5">
         <v>1.14</v>
       </c>
+      <c r="I394" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J394" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -16851,7 +17047,9 @@
       <c r="H395" s="8">
         <v>1.14</v>
       </c>
-      <c r="I395" s="11"/>
+      <c r="I395" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J395" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -16899,6 +17097,9 @@
       <c r="H396" s="5">
         <v>1.34</v>
       </c>
+      <c r="I396" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J396" s="5">
         <f t="shared" si="1"/>
         <v>0.026</v>
@@ -16929,6 +17130,9 @@
       <c r="H397" s="5">
         <v>1.34</v>
       </c>
+      <c r="I397" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J397" s="5">
         <f t="shared" si="1"/>
         <v>0.028</v>
@@ -16959,6 +17163,9 @@
       <c r="H398" s="5">
         <v>1.34</v>
       </c>
+      <c r="I398" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J398" s="5">
         <f t="shared" si="1"/>
         <v>0.027</v>
@@ -16989,7 +17196,9 @@
       <c r="H399" s="8">
         <v>1.34</v>
       </c>
-      <c r="I399" s="11"/>
+      <c r="I399" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J399" s="5">
         <f t="shared" si="1"/>
         <v>0.029</v>
@@ -17037,6 +17246,9 @@
       <c r="H400" s="5">
         <v>1.32</v>
       </c>
+      <c r="I400" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J400" s="5">
         <f t="shared" si="1"/>
         <v>0.03</v>
@@ -17070,6 +17282,9 @@
       <c r="H401" s="5">
         <v>1.32</v>
       </c>
+      <c r="I401" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J401" s="5">
         <f t="shared" si="1"/>
         <v>0.028</v>
@@ -17100,6 +17315,9 @@
       <c r="H402" s="5">
         <v>1.32</v>
       </c>
+      <c r="I402" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J402" s="5">
         <f t="shared" si="1"/>
         <v>0.025</v>
@@ -17130,7 +17348,9 @@
       <c r="H403" s="8">
         <v>1.32</v>
       </c>
-      <c r="I403" s="11"/>
+      <c r="I403" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J403" s="5">
         <f t="shared" si="1"/>
         <v>0.029</v>
@@ -17178,6 +17398,9 @@
       <c r="H404" s="5">
         <v>0.95</v>
       </c>
+      <c r="I404" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J404" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -17208,6 +17431,9 @@
       <c r="H405" s="5">
         <v>0.95</v>
       </c>
+      <c r="I405" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J405" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -17238,6 +17464,9 @@
       <c r="H406" s="5">
         <v>0.95</v>
       </c>
+      <c r="I406" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J406" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -17268,7 +17497,9 @@
       <c r="H407" s="8">
         <v>0.95</v>
       </c>
-      <c r="I407" s="11"/>
+      <c r="I407" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J407" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -17316,6 +17547,9 @@
       <c r="H408" s="5">
         <v>1.17</v>
       </c>
+      <c r="I408" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J408" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -17346,6 +17580,9 @@
       <c r="H409" s="5">
         <v>1.17</v>
       </c>
+      <c r="I409" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J409" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -17376,6 +17613,9 @@
       <c r="H410" s="5">
         <v>1.17</v>
       </c>
+      <c r="I410" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J410" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -17406,7 +17646,9 @@
       <c r="H411" s="8">
         <v>1.17</v>
       </c>
-      <c r="I411" s="11"/>
+      <c r="I411" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J411" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -17454,7 +17696,9 @@
       <c r="H412" s="5">
         <v>1.25</v>
       </c>
-      <c r="I412" s="17"/>
+      <c r="I412" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J412" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -17488,6 +17732,9 @@
       <c r="H413" s="5">
         <v>1.25</v>
       </c>
+      <c r="I413" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J413" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -17518,6 +17765,9 @@
       <c r="H414" s="5">
         <v>1.25</v>
       </c>
+      <c r="I414" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J414" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -17548,7 +17798,9 @@
       <c r="H415" s="8">
         <v>1.25</v>
       </c>
-      <c r="I415" s="11"/>
+      <c r="I415" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J415" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -17596,6 +17848,9 @@
       <c r="H416" s="5">
         <v>1.25</v>
       </c>
+      <c r="I416" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J416" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -17626,6 +17881,9 @@
       <c r="H417" s="5">
         <v>1.25</v>
       </c>
+      <c r="I417" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J417" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -17656,6 +17914,9 @@
       <c r="H418" s="5">
         <v>1.25</v>
       </c>
+      <c r="I418" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J418" s="5">
         <f t="shared" si="1"/>
         <v>0.017</v>
@@ -17686,7 +17947,9 @@
       <c r="H419" s="8">
         <v>1.25</v>
       </c>
-      <c r="I419" s="11"/>
+      <c r="I419" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J419" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -17734,6 +17997,9 @@
       <c r="H420" s="5">
         <v>1.15</v>
       </c>
+      <c r="I420" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J420" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -17764,6 +18030,9 @@
       <c r="H421" s="5">
         <v>1.15</v>
       </c>
+      <c r="I421" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J421" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -17794,6 +18063,9 @@
       <c r="H422" s="5">
         <v>1.15</v>
       </c>
+      <c r="I422" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J422" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -17824,7 +18096,9 @@
       <c r="H423" s="8">
         <v>1.15</v>
       </c>
-      <c r="I423" s="11"/>
+      <c r="I423" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J423" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -17872,6 +18146,9 @@
       <c r="H424" s="5">
         <v>1.17</v>
       </c>
+      <c r="I424" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J424" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -17902,6 +18179,9 @@
       <c r="H425" s="5">
         <v>1.17</v>
       </c>
+      <c r="I425" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J425" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -17932,6 +18212,9 @@
       <c r="H426" s="5">
         <v>1.17</v>
       </c>
+      <c r="I426" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J426" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -17962,7 +18245,9 @@
       <c r="H427" s="8">
         <v>1.17</v>
       </c>
-      <c r="I427" s="11"/>
+      <c r="I427" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J427" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -18010,6 +18295,9 @@
       <c r="H428" s="5">
         <v>1.35</v>
       </c>
+      <c r="I428" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J428" s="5">
         <f t="shared" si="1"/>
         <v>0.035</v>
@@ -18043,6 +18331,9 @@
       <c r="H429" s="5">
         <v>1.35</v>
       </c>
+      <c r="I429" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J429" s="5">
         <f t="shared" si="1"/>
         <v>0.036</v>
@@ -18076,6 +18367,9 @@
       <c r="H430" s="5">
         <v>1.35</v>
       </c>
+      <c r="I430" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J430" s="5">
         <f t="shared" si="1"/>
         <v>0.037</v>
@@ -18109,7 +18403,9 @@
       <c r="H431" s="8">
         <v>1.35</v>
       </c>
-      <c r="I431" s="11"/>
+      <c r="I431" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J431" s="5">
         <f t="shared" si="1"/>
         <v>0.034</v>
@@ -18159,6 +18455,9 @@
       <c r="H432" s="5">
         <v>0.136</v>
       </c>
+      <c r="I432" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J432" s="5">
         <f t="shared" si="1"/>
         <v>0.029</v>
@@ -18192,6 +18491,9 @@
       <c r="H433" s="5">
         <v>0.136</v>
       </c>
+      <c r="I433" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J433" s="5">
         <f t="shared" si="1"/>
         <v>0.032</v>
@@ -18225,6 +18527,9 @@
       <c r="H434" s="5">
         <v>0.136</v>
       </c>
+      <c r="I434" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J434" s="5">
         <f t="shared" si="1"/>
         <v>0.033</v>
@@ -18258,7 +18563,9 @@
       <c r="H435" s="8">
         <v>0.136</v>
       </c>
-      <c r="I435" s="11"/>
+      <c r="I435" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J435" s="5">
         <f t="shared" si="1"/>
         <v>0.03</v>
@@ -18308,6 +18615,9 @@
       <c r="H436" s="5">
         <v>1.16</v>
       </c>
+      <c r="I436" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J436" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -18338,6 +18648,9 @@
       <c r="H437" s="5">
         <v>1.16</v>
       </c>
+      <c r="I437" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J437" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -18368,6 +18681,9 @@
       <c r="H438" s="5">
         <v>1.16</v>
       </c>
+      <c r="I438" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J438" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -18398,7 +18714,9 @@
       <c r="H439" s="8">
         <v>1.16</v>
       </c>
-      <c r="I439" s="11"/>
+      <c r="I439" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J439" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -18446,6 +18764,9 @@
       <c r="H440" s="5">
         <v>1.26</v>
       </c>
+      <c r="I440" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J440" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -18476,6 +18797,9 @@
       <c r="H441" s="5">
         <v>1.26</v>
       </c>
+      <c r="I441" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J441" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -18506,6 +18830,9 @@
       <c r="H442" s="5">
         <v>1.26</v>
       </c>
+      <c r="I442" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J442" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -18536,7 +18863,9 @@
       <c r="H443" s="8">
         <v>1.26</v>
       </c>
-      <c r="I443" s="11"/>
+      <c r="I443" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J443" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -18584,6 +18913,9 @@
       <c r="H444" s="5">
         <v>1.37</v>
       </c>
+      <c r="I444" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J444" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -18614,6 +18946,9 @@
       <c r="H445" s="5">
         <v>1.37</v>
       </c>
+      <c r="I445" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J445" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -18644,6 +18979,9 @@
       <c r="H446" s="5">
         <v>1.37</v>
       </c>
+      <c r="I446" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J446" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -18674,7 +19012,9 @@
       <c r="H447" s="8">
         <v>1.37</v>
       </c>
-      <c r="I447" s="11"/>
+      <c r="I447" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J447" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -18722,6 +19062,9 @@
       <c r="H448" s="5">
         <v>1.4</v>
       </c>
+      <c r="I448" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J448" s="5">
         <f t="shared" si="1"/>
         <v>0.02</v>
@@ -18752,6 +19095,9 @@
       <c r="H449" s="5">
         <v>1.4</v>
       </c>
+      <c r="I449" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J449" s="5">
         <f t="shared" si="1"/>
         <v>0.018</v>
@@ -18782,6 +19128,9 @@
       <c r="H450" s="5">
         <v>1.4</v>
       </c>
+      <c r="I450" s="5">
+        <v>15.0</v>
+      </c>
       <c r="J450" s="5">
         <f t="shared" si="1"/>
         <v>0.021</v>
@@ -18812,7 +19161,9 @@
       <c r="H451" s="8">
         <v>1.4</v>
       </c>
-      <c r="I451" s="11"/>
+      <c r="I451" s="8">
+        <v>15.0</v>
+      </c>
       <c r="J451" s="5">
         <f t="shared" si="1"/>
         <v>0.019</v>
@@ -18860,6 +19211,9 @@
       <c r="H452" s="5">
         <v>0.935</v>
       </c>
+      <c r="I452" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J452" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -18893,6 +19247,9 @@
       <c r="H453" s="5">
         <v>0.935</v>
       </c>
+      <c r="I453" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J453" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -18923,6 +19280,9 @@
       <c r="H454" s="5">
         <v>0.935</v>
       </c>
+      <c r="I454" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J454" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -18953,7 +19313,9 @@
       <c r="H455" s="8">
         <v>0.935</v>
       </c>
-      <c r="I455" s="11"/>
+      <c r="I455" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J455" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -19001,6 +19363,9 @@
       <c r="H456" s="5">
         <v>0.985</v>
       </c>
+      <c r="I456" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J456" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -19031,6 +19396,9 @@
       <c r="H457" s="5">
         <v>0.985</v>
       </c>
+      <c r="I457" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J457" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -19061,6 +19429,9 @@
       <c r="H458" s="5">
         <v>0.985</v>
       </c>
+      <c r="I458" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J458" s="5">
         <f t="shared" si="1"/>
         <v>0.016</v>
@@ -19091,7 +19462,9 @@
       <c r="H459" s="8">
         <v>0.985</v>
       </c>
-      <c r="I459" s="11"/>
+      <c r="I459" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J459" s="5">
         <f t="shared" si="1"/>
         <v>0.017</v>
@@ -19139,6 +19512,9 @@
       <c r="H460" s="5">
         <v>1.335</v>
       </c>
+      <c r="I460" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J460" s="5">
         <f t="shared" si="1"/>
         <v>0.025</v>
@@ -19169,6 +19545,9 @@
       <c r="H461" s="5">
         <v>1.335</v>
       </c>
+      <c r="I461" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J461" s="5">
         <f t="shared" si="1"/>
         <v>0.025</v>
@@ -19199,6 +19578,9 @@
       <c r="H462" s="5">
         <v>1.335</v>
       </c>
+      <c r="I462" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J462" s="5">
         <f t="shared" si="1"/>
         <v>0.025</v>
@@ -19229,7 +19611,9 @@
       <c r="H463" s="8">
         <v>1.335</v>
       </c>
-      <c r="I463" s="11"/>
+      <c r="I463" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J463" s="5">
         <f t="shared" si="1"/>
         <v>0.024</v>
@@ -19277,6 +19661,9 @@
       <c r="H464" s="5">
         <v>1.24</v>
       </c>
+      <c r="I464" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J464" s="5">
         <f t="shared" si="1"/>
         <v>0.034</v>
@@ -19307,6 +19694,9 @@
       <c r="H465" s="5">
         <v>1.24</v>
       </c>
+      <c r="I465" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J465" s="5">
         <f t="shared" si="1"/>
         <v>0.037</v>
@@ -19337,6 +19727,9 @@
       <c r="H466" s="5">
         <v>1.24</v>
       </c>
+      <c r="I466" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J466" s="5">
         <f t="shared" si="1"/>
         <v>0.024</v>
@@ -19367,7 +19760,9 @@
       <c r="H467" s="8">
         <v>1.24</v>
       </c>
-      <c r="I467" s="11"/>
+      <c r="I467" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J467" s="5">
         <f t="shared" si="1"/>
         <v>0.024</v>
@@ -19415,6 +19810,9 @@
       <c r="H468" s="5">
         <v>1.15</v>
       </c>
+      <c r="I468" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J468" s="5">
         <f t="shared" si="1"/>
         <v>0.019</v>
@@ -19445,6 +19843,9 @@
       <c r="H469" s="5">
         <v>1.15</v>
       </c>
+      <c r="I469" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J469" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -19475,6 +19876,9 @@
       <c r="H470" s="5">
         <v>1.15</v>
       </c>
+      <c r="I470" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J470" s="5">
         <f t="shared" si="1"/>
         <v>-0.004</v>
@@ -19508,7 +19912,9 @@
       <c r="H471" s="8">
         <v>1.15</v>
       </c>
-      <c r="I471" s="11"/>
+      <c r="I471" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J471" s="5">
         <f t="shared" si="1"/>
         <v>0.015</v>
@@ -19556,6 +19962,9 @@
       <c r="H472" s="5">
         <v>1.1</v>
       </c>
+      <c r="I472" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J472" s="5">
         <f t="shared" si="1"/>
         <v>0.008</v>
@@ -19586,6 +19995,9 @@
       <c r="H473" s="5">
         <v>1.1</v>
       </c>
+      <c r="I473" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J473" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -19616,6 +20028,9 @@
       <c r="H474" s="5">
         <v>1.1</v>
       </c>
+      <c r="I474" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J474" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -19646,7 +20061,9 @@
       <c r="H475" s="8">
         <v>1.1</v>
       </c>
-      <c r="I475" s="11"/>
+      <c r="I475" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J475" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -19694,6 +20111,9 @@
       <c r="H476" s="5">
         <v>1.35</v>
       </c>
+      <c r="I476" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J476" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -19724,6 +20144,9 @@
       <c r="H477" s="5">
         <v>1.35</v>
       </c>
+      <c r="I477" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J477" s="5">
         <f t="shared" si="1"/>
         <v>0.008</v>
@@ -19754,6 +20177,9 @@
       <c r="H478" s="5">
         <v>1.35</v>
       </c>
+      <c r="I478" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J478" s="5">
         <f t="shared" si="1"/>
         <v>0.008</v>
@@ -19784,7 +20210,9 @@
       <c r="H479" s="8">
         <v>1.35</v>
       </c>
-      <c r="I479" s="11"/>
+      <c r="I479" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J479" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -19832,6 +20260,9 @@
       <c r="H480" s="5">
         <v>1.25</v>
       </c>
+      <c r="I480" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J480" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -19862,6 +20293,9 @@
       <c r="H481" s="5">
         <v>1.25</v>
       </c>
+      <c r="I481" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J481" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -19892,6 +20326,9 @@
       <c r="H482" s="5">
         <v>1.25</v>
       </c>
+      <c r="I482" s="5">
+        <v>13.0</v>
+      </c>
       <c r="J482" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -19922,7 +20359,9 @@
       <c r="H483" s="8">
         <v>1.25</v>
       </c>
-      <c r="I483" s="11"/>
+      <c r="I483" s="8">
+        <v>13.0</v>
+      </c>
       <c r="J483" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -19970,6 +20409,9 @@
       <c r="H484" s="5">
         <v>1.33</v>
       </c>
+      <c r="I484" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J484" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -19997,7 +20439,12 @@
       <c r="G485" s="5">
         <v>0.099</v>
       </c>
-      <c r="H485" s="17"/>
+      <c r="H485" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="I485" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J485" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -20025,7 +20472,12 @@
       <c r="G486" s="5">
         <v>0.099</v>
       </c>
-      <c r="H486" s="17"/>
+      <c r="H486" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="I486" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J486" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -20053,8 +20505,12 @@
       <c r="G487" s="8">
         <v>0.097</v>
       </c>
-      <c r="H487" s="11"/>
-      <c r="I487" s="11"/>
+      <c r="H487" s="8">
+        <v>1.33</v>
+      </c>
+      <c r="I487" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J487" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -20102,6 +20558,9 @@
       <c r="H488" s="5">
         <v>1.39</v>
       </c>
+      <c r="I488" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J488" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -20129,7 +20588,12 @@
       <c r="G489" s="5">
         <v>0.099</v>
       </c>
-      <c r="H489" s="17"/>
+      <c r="H489" s="5">
+        <v>1.39</v>
+      </c>
+      <c r="I489" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J489" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -20157,7 +20621,12 @@
       <c r="G490" s="5">
         <v>0.099</v>
       </c>
-      <c r="H490" s="17"/>
+      <c r="H490" s="5">
+        <v>1.39</v>
+      </c>
+      <c r="I490" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J490" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -20185,8 +20654,12 @@
       <c r="G491" s="8">
         <v>0.099</v>
       </c>
-      <c r="H491" s="11"/>
-      <c r="I491" s="11"/>
+      <c r="H491" s="8">
+        <v>1.39</v>
+      </c>
+      <c r="I491" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J491" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -20234,6 +20707,9 @@
       <c r="H492" s="5">
         <v>1.425</v>
       </c>
+      <c r="I492" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J492" s="5">
         <f t="shared" si="1"/>
         <v>0.027</v>
@@ -20261,7 +20737,12 @@
       <c r="G493" s="5">
         <v>0.08</v>
       </c>
-      <c r="H493" s="17"/>
+      <c r="H493" s="5">
+        <v>1.425</v>
+      </c>
+      <c r="I493" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J493" s="5">
         <f t="shared" si="1"/>
         <v>0.027</v>
@@ -20289,7 +20770,12 @@
       <c r="G494" s="5">
         <v>0.08</v>
       </c>
-      <c r="H494" s="17"/>
+      <c r="H494" s="5">
+        <v>1.425</v>
+      </c>
+      <c r="I494" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J494" s="5">
         <f t="shared" si="1"/>
         <v>0.026</v>
@@ -20317,8 +20803,12 @@
       <c r="G495" s="8">
         <v>0.08</v>
       </c>
-      <c r="H495" s="11"/>
-      <c r="I495" s="11"/>
+      <c r="H495" s="8">
+        <v>1.425</v>
+      </c>
+      <c r="I495" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J495" s="5">
         <f t="shared" si="1"/>
         <v>0.027</v>
@@ -20366,6 +20856,9 @@
       <c r="H496" s="5">
         <v>1.49</v>
       </c>
+      <c r="I496" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J496" s="5">
         <f t="shared" si="1"/>
         <v>0.024</v>
@@ -20393,7 +20886,12 @@
       <c r="G497" s="5">
         <v>0.08</v>
       </c>
-      <c r="H497" s="17"/>
+      <c r="H497" s="5">
+        <v>1.49</v>
+      </c>
+      <c r="I497" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J497" s="5">
         <f t="shared" si="1"/>
         <v>0.024</v>
@@ -20421,7 +20919,12 @@
       <c r="G498" s="5">
         <v>0.081</v>
       </c>
-      <c r="H498" s="17"/>
+      <c r="H498" s="5">
+        <v>1.49</v>
+      </c>
+      <c r="I498" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J498" s="5">
         <f t="shared" si="1"/>
         <v>0.024</v>
@@ -20449,8 +20952,12 @@
       <c r="G499" s="8">
         <v>0.08</v>
       </c>
-      <c r="H499" s="11"/>
-      <c r="I499" s="11"/>
+      <c r="H499" s="8">
+        <v>1.49</v>
+      </c>
+      <c r="I499" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J499" s="5">
         <f t="shared" si="1"/>
         <v>0.022</v>
@@ -20498,6 +21005,9 @@
       <c r="H500" s="5">
         <v>1.14</v>
       </c>
+      <c r="I500" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J500" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -20525,7 +21035,12 @@
       <c r="G501" s="5">
         <v>0.149</v>
       </c>
-      <c r="H501" s="17"/>
+      <c r="H501" s="5">
+        <v>1.14</v>
+      </c>
+      <c r="I501" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J501" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -20553,7 +21068,12 @@
       <c r="G502" s="5">
         <v>0.15</v>
       </c>
-      <c r="H502" s="17"/>
+      <c r="H502" s="5">
+        <v>1.14</v>
+      </c>
+      <c r="I502" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J502" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -20581,8 +21101,12 @@
       <c r="G503" s="8">
         <v>0.149</v>
       </c>
-      <c r="H503" s="11"/>
-      <c r="I503" s="11"/>
+      <c r="H503" s="8">
+        <v>1.14</v>
+      </c>
+      <c r="I503" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J503" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -20630,6 +21154,9 @@
       <c r="H504" s="5">
         <v>1.16</v>
       </c>
+      <c r="I504" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J504" s="5">
         <f t="shared" si="1"/>
         <v>0.004</v>
@@ -20657,7 +21184,12 @@
       <c r="G505" s="5">
         <v>0.15</v>
       </c>
-      <c r="H505" s="17"/>
+      <c r="H505" s="5">
+        <v>1.16</v>
+      </c>
+      <c r="I505" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J505" s="5">
         <f t="shared" si="1"/>
         <v>0.004</v>
@@ -20685,7 +21217,12 @@
       <c r="G506" s="5">
         <v>0.15</v>
       </c>
-      <c r="H506" s="17"/>
+      <c r="H506" s="5">
+        <v>1.16</v>
+      </c>
+      <c r="I506" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J506" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -20713,8 +21250,12 @@
       <c r="G507" s="8">
         <v>0.151</v>
       </c>
-      <c r="H507" s="11"/>
-      <c r="I507" s="11"/>
+      <c r="H507" s="8">
+        <v>1.16</v>
+      </c>
+      <c r="I507" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J507" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -20762,6 +21303,9 @@
       <c r="H508" s="5">
         <v>1.39</v>
       </c>
+      <c r="I508" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J508" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -20789,7 +21333,12 @@
       <c r="G509" s="5">
         <v>0.102</v>
       </c>
-      <c r="H509" s="17"/>
+      <c r="H509" s="5">
+        <v>1.39</v>
+      </c>
+      <c r="I509" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J509" s="5">
         <f t="shared" si="1"/>
         <v>0.005</v>
@@ -20817,7 +21366,12 @@
       <c r="G510" s="5">
         <v>0.102</v>
       </c>
-      <c r="H510" s="17"/>
+      <c r="H510" s="5">
+        <v>1.39</v>
+      </c>
+      <c r="I510" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J510" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -20845,8 +21399,12 @@
       <c r="G511" s="8">
         <v>0.1</v>
       </c>
-      <c r="H511" s="11"/>
-      <c r="I511" s="11"/>
+      <c r="H511" s="8">
+        <v>1.39</v>
+      </c>
+      <c r="I511" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J511" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -20894,6 +21452,9 @@
       <c r="H512" s="5">
         <v>1.37</v>
       </c>
+      <c r="I512" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J512" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -20921,7 +21482,12 @@
       <c r="G513" s="5">
         <v>0.099</v>
       </c>
-      <c r="H513" s="17"/>
+      <c r="H513" s="5">
+        <v>1.37</v>
+      </c>
+      <c r="I513" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J513" s="5">
         <f t="shared" si="1"/>
         <v>0.008</v>
@@ -20949,7 +21515,12 @@
       <c r="G514" s="5">
         <v>0.1</v>
       </c>
-      <c r="H514" s="17"/>
+      <c r="H514" s="5">
+        <v>1.37</v>
+      </c>
+      <c r="I514" s="5">
+        <v>11.0</v>
+      </c>
       <c r="J514" s="5">
         <f t="shared" si="1"/>
         <v>0.006</v>
@@ -20977,8 +21548,12 @@
       <c r="G515" s="8">
         <v>0.101</v>
       </c>
-      <c r="H515" s="11"/>
-      <c r="I515" s="11"/>
+      <c r="H515" s="8">
+        <v>1.37</v>
+      </c>
+      <c r="I515" s="8">
+        <v>11.0</v>
+      </c>
       <c r="J515" s="5">
         <f t="shared" si="1"/>
         <v>0.007</v>
@@ -21026,6 +21601,9 @@
       <c r="H516" s="5">
         <v>1.085</v>
       </c>
+      <c r="I516" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J516" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -21053,7 +21631,12 @@
       <c r="G517" s="5">
         <v>0.15</v>
       </c>
-      <c r="H517" s="17"/>
+      <c r="H517" s="5">
+        <v>1.085</v>
+      </c>
+      <c r="I517" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J517" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -21081,7 +21664,12 @@
       <c r="G518" s="5">
         <v>0.151</v>
       </c>
-      <c r="H518" s="17"/>
+      <c r="H518" s="5">
+        <v>1.085</v>
+      </c>
+      <c r="I518" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J518" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -21109,8 +21697,12 @@
       <c r="G519" s="8">
         <v>0.15</v>
       </c>
-      <c r="H519" s="11"/>
-      <c r="I519" s="11"/>
+      <c r="H519" s="8">
+        <v>1.085</v>
+      </c>
+      <c r="I519" s="8">
+        <v>17.0</v>
+      </c>
       <c r="J519" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -21158,6 +21750,9 @@
       <c r="H520" s="5">
         <v>1.335</v>
       </c>
+      <c r="I520" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J520" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -21185,7 +21780,12 @@
       <c r="G521" s="5">
         <v>0.1</v>
       </c>
-      <c r="H521" s="17"/>
+      <c r="H521" s="5">
+        <v>1.335</v>
+      </c>
+      <c r="I521" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J521" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -21213,7 +21813,12 @@
       <c r="G522" s="5">
         <v>0.99</v>
       </c>
-      <c r="H522" s="17"/>
+      <c r="H522" s="5">
+        <v>1.335</v>
+      </c>
+      <c r="I522" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J522" s="5">
         <f t="shared" si="1"/>
         <v>0.012</v>
@@ -21241,8 +21846,12 @@
       <c r="G523" s="8">
         <v>0.99</v>
       </c>
-      <c r="H523" s="11"/>
-      <c r="I523" s="11"/>
+      <c r="H523" s="8">
+        <v>1.335</v>
+      </c>
+      <c r="I523" s="8">
+        <v>17.0</v>
+      </c>
       <c r="J523" s="5">
         <f t="shared" si="1"/>
         <v>0.009</v>
@@ -21290,6 +21899,9 @@
       <c r="H524" s="5">
         <v>1.385</v>
       </c>
+      <c r="I524" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J524" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -21317,7 +21929,12 @@
       <c r="G525" s="5">
         <v>0.1</v>
       </c>
-      <c r="H525" s="17"/>
+      <c r="H525" s="5">
+        <v>1.385</v>
+      </c>
+      <c r="I525" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J525" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -21345,7 +21962,12 @@
       <c r="G526" s="5">
         <v>0.1</v>
       </c>
-      <c r="H526" s="17"/>
+      <c r="H526" s="5">
+        <v>1.385</v>
+      </c>
+      <c r="I526" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J526" s="5">
         <f t="shared" si="1"/>
         <v>0.013</v>
@@ -21373,8 +21995,12 @@
       <c r="G527" s="5">
         <v>0.1</v>
       </c>
-      <c r="H527" s="11"/>
-      <c r="I527" s="11"/>
+      <c r="H527" s="8">
+        <v>1.385</v>
+      </c>
+      <c r="I527" s="8">
+        <v>17.0</v>
+      </c>
       <c r="J527" s="5">
         <f t="shared" si="1"/>
         <v>0.014</v>
@@ -21422,6 +22048,9 @@
       <c r="H528" s="5">
         <v>1.375</v>
       </c>
+      <c r="I528" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J528" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -21452,6 +22081,9 @@
       <c r="H529" s="5">
         <v>1.375</v>
       </c>
+      <c r="I529" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J529" s="5">
         <f t="shared" si="1"/>
         <v>0.011</v>
@@ -21482,6 +22114,9 @@
       <c r="H530" s="5">
         <v>1.375</v>
       </c>
+      <c r="I530" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J530" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -21512,7 +22147,9 @@
       <c r="H531" s="5">
         <v>1.375</v>
       </c>
-      <c r="I531" s="11"/>
+      <c r="I531" s="8">
+        <v>17.0</v>
+      </c>
       <c r="J531" s="5">
         <f t="shared" si="1"/>
         <v>0.01</v>
@@ -21560,6 +22197,9 @@
       <c r="H532" s="5">
         <v>1.13</v>
       </c>
+      <c r="I532" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J532" s="5">
         <f t="shared" si="1"/>
         <v>0.026</v>
@@ -21590,6 +22230,9 @@
       <c r="H533" s="5">
         <v>1.13</v>
       </c>
+      <c r="I533" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J533" s="5">
         <f t="shared" si="1"/>
         <v>0.026</v>
@@ -21620,6 +22263,9 @@
       <c r="H534" s="5">
         <v>1.13</v>
       </c>
+      <c r="I534" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J534" s="5">
         <f t="shared" si="1"/>
         <v>0.026</v>
@@ -21650,7 +22296,9 @@
       <c r="H535" s="5">
         <v>1.13</v>
       </c>
-      <c r="I535" s="11"/>
+      <c r="I535" s="8">
+        <v>17.0</v>
+      </c>
       <c r="J535" s="5">
         <f t="shared" si="1"/>
         <v>0.027</v>
@@ -21698,6 +22346,9 @@
       <c r="H536" s="5">
         <v>1.15</v>
       </c>
+      <c r="I536" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J536" s="5">
         <f t="shared" si="1"/>
         <v>0.028</v>
@@ -21728,6 +22379,9 @@
       <c r="H537" s="5">
         <v>1.15</v>
       </c>
+      <c r="I537" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J537" s="5">
         <f t="shared" si="1"/>
         <v>0.026</v>
@@ -21758,6 +22412,9 @@
       <c r="H538" s="5">
         <v>1.15</v>
       </c>
+      <c r="I538" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J538" s="5">
         <f t="shared" si="1"/>
         <v>0.028</v>
@@ -21788,7 +22445,9 @@
       <c r="H539" s="5">
         <v>1.15</v>
       </c>
-      <c r="I539" s="11"/>
+      <c r="I539" s="8">
+        <v>17.0</v>
+      </c>
       <c r="J539" s="5">
         <f t="shared" si="1"/>
         <v>0.026</v>
@@ -21836,6 +22495,9 @@
       <c r="H540" s="5">
         <v>1.35</v>
       </c>
+      <c r="I540" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J540" s="5">
         <f t="shared" si="1"/>
         <v>0.038</v>
@@ -21866,6 +22528,9 @@
       <c r="H541" s="5">
         <v>1.35</v>
       </c>
+      <c r="I541" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J541" s="5">
         <f t="shared" si="1"/>
         <v>0.033</v>
@@ -21896,6 +22561,9 @@
       <c r="H542" s="5">
         <v>1.35</v>
       </c>
+      <c r="I542" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J542" s="5">
         <f t="shared" si="1"/>
         <v>0.037</v>
@@ -21926,6 +22594,9 @@
       <c r="H543" s="5">
         <v>1.35</v>
       </c>
+      <c r="I543" s="8">
+        <v>17.0</v>
+      </c>
       <c r="J543" s="5">
         <f t="shared" si="1"/>
         <v>0.036</v>
@@ -21956,6 +22627,9 @@
       <c r="H544" s="5">
         <v>1.3</v>
       </c>
+      <c r="I544" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J544" s="5">
         <f t="shared" si="1"/>
         <v>0.037</v>
@@ -21986,6 +22660,9 @@
       <c r="H545" s="5">
         <v>1.3</v>
       </c>
+      <c r="I545" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J545" s="5">
         <f t="shared" si="1"/>
         <v>0.033</v>
@@ -22016,6 +22693,9 @@
       <c r="H546" s="5">
         <v>1.3</v>
       </c>
+      <c r="I546" s="5">
+        <v>17.0</v>
+      </c>
       <c r="J546" s="5">
         <f t="shared" si="1"/>
         <v>0.034</v>
@@ -22045,6 +22725,9 @@
       </c>
       <c r="H547" s="5">
         <v>1.3</v>
+      </c>
+      <c r="I547" s="8">
+        <v>17.0</v>
       </c>
       <c r="J547" s="5">
         <f t="shared" si="1"/>
@@ -25009,7 +25692,7 @@
     <dataValidation type="list" allowBlank="1" showDropDown="1" sqref="C4:C5">
       <formula1>"B_sed_4m_R1_F1,B_sed_4m_R1_F2"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" sqref="H4:H267 H271:H411 H412:I412 K412 H413:H487 H489:H967">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" sqref="H4:H267 K412 H271:H487 H492:H967">
       <formula1>0.985</formula1>
       <formula2>1.573</formula2>
     </dataValidation>

</xml_diff>